<commit_message>
Add form domisili and jampersal
</commit_message>
<xml_diff>
--- a/assets/form/testing2.xlsx
+++ b/assets/form/testing2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programs\xampp\htdocs\newsid\assets\form\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310CC133-A2A9-4EF4-9934-9F1D3F1C1B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2470C5-C1EC-4227-B552-A5A9B4D386F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3488242F-0895-47DD-9472-A3A624CCB03D}"/>
   </bookViews>
@@ -92,10 +92,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -111,6 +111,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32915E55-2396-4ED0-BDAE-E3473D5388AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="441960" y="914400"/>
+          <a:ext cx="3451860" cy="198120"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,43 +468,43 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -457,5 +512,6 @@
     <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>